<commit_message>
ugprade POI 5.1, upgrade dependencies
</commit_message>
<xml_diff>
--- a/hiveserde/src/test/resources/testdata/testsimple.xlsx
+++ b/hiveserde/src/test/resources/testdata/testsimple.xlsx
@@ -1,23 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/tmp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jornfranke/repos/work/hadoopoffice/flinkds/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F7B900-7FB9-584F-AC95-B525C3FD992B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19420" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -77,10 +87,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;WAHR&quot;;&quot;WAHR&quot;;&quot;FALSCH&quot;"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -114,17 +124,20 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -392,10 +405,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -456,7 +471,7 @@
       <c r="G2" s="3">
         <v>3</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="3">
         <v>100</v>
       </c>
       <c r="I2" s="3">
@@ -486,7 +501,7 @@
       <c r="G3" s="3">
         <v>4</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="3">
         <v>65335</v>
       </c>
       <c r="I3" s="3">
@@ -515,7 +530,7 @@
       <c r="G4" s="3">
         <v>5</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="3">
         <v>1</v>
       </c>
       <c r="I4" s="3">
@@ -544,7 +559,7 @@
       <c r="G5" s="3">
         <v>250</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <v>250</v>
       </c>
       <c r="I5" s="3">
@@ -566,7 +581,7 @@
       <c r="G6" s="3">
         <v>3</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="3">
         <v>5</v>
       </c>
       <c r="I6" s="3">
@@ -595,7 +610,7 @@
       <c r="G7" s="3">
         <v>100</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <v>10000</v>
       </c>
       <c r="I7" s="3">

</xml_diff>